<commit_message>
Finish validation function for local access and add function to get daily acquisition numbers/totals
</commit_message>
<xml_diff>
--- a/qcdata/PARAMETERS.xlsx
+++ b/qcdata/PARAMETERS.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\PP3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DF0B63C-92B1-44BC-9832-5B7E635C2630}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6BE4599-B8A6-47E0-910C-976D927B064A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="780" windowWidth="20895" windowHeight="14115" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6630" yWindow="1155" windowWidth="20895" windowHeight="14115" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tolerances" sheetId="1" r:id="rId1"/>
@@ -56,16 +56,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
-      <name val="Arial"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="10"/>
-      <color theme="4"/>
       <name val="Arial"/>
     </font>
     <font>
@@ -99,11 +93,6 @@
       <color rgb="FF4285F4"/>
       <name val="Arial"/>
     </font>
-    <font>
-      <sz val="10"/>
-      <color theme="4"/>
-      <name val="Arial"/>
-    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -269,56 +258,54 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -539,117 +526,101 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:E11"/>
+  <dimension ref="B2:E11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="4.42578125" customWidth="1"/>
+    <col min="1" max="1" width="4.5703125" customWidth="1"/>
     <col min="2" max="2" width="52" customWidth="1"/>
     <col min="3" max="5" width="26.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" s="1"/>
-      <c r="B1" s="1"/>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" s="1"/>
-      <c r="B2" s="2" t="s">
+    <row r="2" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="E2" s="4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" s="1"/>
-      <c r="B3" s="6" t="s">
+    <row r="3" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B3" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="7">
+      <c r="C3" s="6">
         <v>2</v>
       </c>
-      <c r="D3" s="8"/>
-      <c r="E3" s="9"/>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" s="1"/>
-      <c r="B4" s="10" t="s">
+      <c r="D3" s="7"/>
+      <c r="E3" s="8"/>
+    </row>
+    <row r="4" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B4" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="11">
+      <c r="C4" s="10">
         <v>4</v>
       </c>
-      <c r="E4" s="12"/>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" s="1"/>
-      <c r="B5" s="13"/>
-      <c r="C5" s="14"/>
-      <c r="D5" s="15"/>
-      <c r="E5" s="16"/>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" s="1"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" s="1"/>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8" s="1"/>
-      <c r="B8" s="2" t="s">
+      <c r="E4" s="11"/>
+    </row>
+    <row r="5" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B5" s="12"/>
+      <c r="C5" s="13"/>
+      <c r="D5" s="14"/>
+      <c r="E5" s="15"/>
+    </row>
+    <row r="8" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B8" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C8" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D8" s="4" t="s">
+      <c r="D8" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E8" s="5" t="s">
+      <c r="E8" s="4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9" s="17"/>
-      <c r="B9" s="6" t="s">
+    <row r="9" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B9" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C9" s="7">
+      <c r="C9" s="6">
         <v>1</v>
       </c>
-      <c r="D9" s="18"/>
-      <c r="E9" s="19"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" s="17"/>
-      <c r="B10" s="6" t="s">
+      <c r="D9" s="16"/>
+      <c r="E9" s="17"/>
+    </row>
+    <row r="10" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B10" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="7">
+      <c r="C10" s="6">
         <v>10</v>
       </c>
-      <c r="D10" s="20"/>
-      <c r="E10" s="21"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11" s="17"/>
-      <c r="B11" s="13" t="s">
+      <c r="D10" s="18"/>
+      <c r="E10" s="19"/>
+    </row>
+    <row r="11" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B11" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="C11" s="22"/>
-      <c r="D11" s="23">
+      <c r="C11" s="20"/>
+      <c r="D11" s="21">
         <v>70</v>
       </c>
-      <c r="E11" s="24">
+      <c r="E11" s="22">
         <v>80</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Detect and correct missing option to give the user the opportunity to enter acquisition parameters if the corresponding file exists but a value is missing, for both Google Drive and local options
</commit_message>
<xml_diff>
--- a/qcdata/PARAMETERS.xlsx
+++ b/qcdata/PARAMETERS.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\PP3\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\z_Others\2021_Code_Institute\Software_Developer\Milestone_Project_3\PP3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6BE4599-B8A6-47E0-910C-976D927B064A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBEA5421-10C2-46DC-AF06-6A73DBF1D6A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6630" yWindow="1155" windowWidth="20895" windowHeight="14115" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tolerances" sheetId="1" r:id="rId1"/>
@@ -529,7 +529,7 @@
   <dimension ref="B2:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -596,9 +596,7 @@
       <c r="B9" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C9" s="6">
-        <v>1</v>
-      </c>
+      <c r="C9" s="6"/>
       <c r="D9" s="16"/>
       <c r="E9" s="17"/>
     </row>

</xml_diff>

<commit_message>
Correct print message with spaces in run.py, validate run.py and functions.py with PEP8, and add evidence images to README.md
</commit_message>
<xml_diff>
--- a/qcdata/PARAMETERS.xlsx
+++ b/qcdata/PARAMETERS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\z_Others\2021_Code_Institute\Software_Developer\Milestone_Project_3\PP3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBEA5421-10C2-46DC-AF06-6A73DBF1D6A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35C4FEE7-B629-48AE-B647-4087253F3C06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -529,7 +529,7 @@
   <dimension ref="B2:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -596,7 +596,9 @@
       <c r="B9" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C9" s="6"/>
+      <c r="C9" s="6">
+        <v>1</v>
+      </c>
       <c r="D9" s="16"/>
       <c r="E9" s="17"/>
     </row>

</xml_diff>

<commit_message>
Add checking of missing data when computing points to reacquire, correct minor details in README.md file, recheck functions.py with PEP8, update evidence image, and check with different content/names in/of the files, for testing.
</commit_message>
<xml_diff>
--- a/qcdata/PARAMETERS.xlsx
+++ b/qcdata/PARAMETERS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\z_Others\2021_Code_Institute\Software_Developer\Milestone_Project_3\PP3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2381429D-DFE3-4117-9308-A47893FDC3FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F10EE8A0-BD72-4F16-8B5F-BEE5C75925DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -529,7 +529,7 @@
   <dimension ref="B2:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -617,7 +617,9 @@
         <v>9</v>
       </c>
       <c r="C11" s="20"/>
-      <c r="D11" s="21"/>
+      <c r="D11" s="21">
+        <v>70</v>
+      </c>
       <c r="E11" s="22">
         <v>80</v>
       </c>

</xml_diff>